<commit_message>
updated E-W data spreadsheet
</commit_message>
<xml_diff>
--- a/E-W data.xlsx
+++ b/E-W data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mikael\Documents\Zimanyi group\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1B324D-84B3-4AD3-A3B0-BDFD3D0859EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E564DCF9-12FF-445C-96AB-689509F71389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16710" yWindow="2730" windowWidth="20085" windowHeight="17220" xr2:uid="{65DA8866-190D-4A07-B9F8-06CAA00B3B4B}"/>
+    <workbookView xWindow="2940" yWindow="75" windowWidth="20085" windowHeight="17385" xr2:uid="{65DA8866-190D-4A07-B9F8-06CAA00B3B4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="58">
   <si>
     <t>File</t>
   </si>
@@ -160,6 +160,54 @@
   </si>
   <si>
     <t>E2W6.png</t>
+  </si>
+  <si>
+    <t>1.356 [.302, .398]</t>
+  </si>
+  <si>
+    <t>1.326 [.261, .371]</t>
+  </si>
+  <si>
+    <t>1.702 [.574, .891]</t>
+  </si>
+  <si>
+    <t>offdiagE6W15HRCombined.txt</t>
+  </si>
+  <si>
+    <t>1.443 [.331, .523]</t>
+  </si>
+  <si>
+    <t>E6W15HRCombined.png</t>
+  </si>
+  <si>
+    <t>1.142 [.117, .167]</t>
+  </si>
+  <si>
+    <t>1.177 [.150, .206]</t>
+  </si>
+  <si>
+    <t>1.253 [.196, .306]</t>
+  </si>
+  <si>
+    <t>1.368 [.187, .528]</t>
+  </si>
+  <si>
+    <t>1.182 [.160, .205]</t>
+  </si>
+  <si>
+    <t>1.201 [.174, .230]</t>
+  </si>
+  <si>
+    <t>1.225 [.134, .271]</t>
+  </si>
+  <si>
+    <t>1.382 [.272, .445]</t>
+  </si>
+  <si>
+    <t>1.484 [.390, .588]</t>
+  </si>
+  <si>
+    <t>1.105 [.985, .044]</t>
   </si>
 </sst>
 </file>
@@ -599,12 +647,13 @@
   <dimension ref="A1:R70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" customWidth="1"/>
   </cols>
@@ -636,11 +685,11 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
-        <v>1.145</v>
+      <c r="B2" t="s">
+        <v>48</v>
       </c>
       <c r="C2">
-        <v>0.3</v>
+        <v>0.31</v>
       </c>
       <c r="D2">
         <v>3121</v>
@@ -653,8 +702,8 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>1.175</v>
+      <c r="B3" t="s">
+        <v>49</v>
       </c>
       <c r="C3">
         <v>0.44</v>
@@ -670,11 +719,11 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>1.254</v>
+      <c r="B4" t="s">
+        <v>50</v>
       </c>
       <c r="C4">
-        <v>0.57999999999999996</v>
+        <v>0.58599999999999997</v>
       </c>
       <c r="D4">
         <v>3121</v>
@@ -687,11 +736,11 @@
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
-        <v>1.3220000000000001</v>
+      <c r="B5" t="s">
+        <v>51</v>
       </c>
       <c r="C5">
-        <v>0.74</v>
+        <v>0.76400000000000001</v>
       </c>
       <c r="D5">
         <v>3121</v>
@@ -704,11 +753,11 @@
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6">
-        <v>1.1819999999999999</v>
+      <c r="B6" t="s">
+        <v>52</v>
       </c>
       <c r="C6">
-        <v>0.39</v>
+        <v>0.38600000000000001</v>
       </c>
       <c r="D6">
         <v>3121</v>
@@ -721,11 +770,11 @@
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7">
-        <v>1.204</v>
+      <c r="B7" t="s">
+        <v>53</v>
       </c>
       <c r="C7">
-        <v>0.49</v>
+        <v>0.49199999999999999</v>
       </c>
       <c r="D7">
         <v>3121</v>
@@ -738,11 +787,11 @@
       <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B8">
-        <v>1.228</v>
+      <c r="B8" t="s">
+        <v>54</v>
       </c>
       <c r="C8">
-        <v>0.62</v>
+        <v>0.621</v>
       </c>
       <c r="D8">
         <v>3121</v>
@@ -755,11 +804,11 @@
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B9">
-        <v>1.4970000000000001</v>
+      <c r="B9" t="s">
+        <v>56</v>
       </c>
       <c r="C9">
-        <v>0.79</v>
+        <v>0.79100000000000004</v>
       </c>
       <c r="D9">
         <v>3121</v>
@@ -772,11 +821,11 @@
       <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B10">
-        <v>1.3560000000000001</v>
+      <c r="B10" t="s">
+        <v>42</v>
       </c>
       <c r="C10">
-        <v>0.64</v>
+        <v>0.63500000000000001</v>
       </c>
       <c r="D10">
         <v>3121</v>
@@ -789,8 +838,8 @@
       <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B11">
-        <v>1.327</v>
+      <c r="B11" t="s">
+        <v>43</v>
       </c>
       <c r="C11">
         <v>0.64</v>
@@ -806,11 +855,11 @@
       <c r="A12" t="s">
         <v>14</v>
       </c>
-      <c r="B12">
-        <v>1.3859999999999999</v>
+      <c r="B12" t="s">
+        <v>55</v>
       </c>
       <c r="C12">
-        <v>0.74</v>
+        <v>0.74299999999999999</v>
       </c>
       <c r="D12">
         <v>3121</v>
@@ -823,11 +872,11 @@
       <c r="A13" t="s">
         <v>15</v>
       </c>
-      <c r="B13">
-        <v>1.849</v>
+      <c r="B13" t="s">
+        <v>44</v>
       </c>
       <c r="C13">
-        <v>0.88</v>
+        <v>0.88300000000000001</v>
       </c>
       <c r="D13">
         <v>3121</v>
@@ -840,8 +889,8 @@
       <c r="A14" t="s">
         <v>40</v>
       </c>
-      <c r="B14">
-        <v>1.01</v>
+      <c r="B14" t="s">
+        <v>57</v>
       </c>
       <c r="C14">
         <v>6.0999999999999999E-2</v>
@@ -851,6 +900,23 @@
       </c>
       <c r="E14" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15">
+        <v>0.8</v>
+      </c>
+      <c r="D15">
+        <v>3121</v>
+      </c>
+      <c r="E15" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="9:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added E5W10 data and updated E-W spreadsheet updated E0W8 data
</commit_message>
<xml_diff>
--- a/E-W data.xlsx
+++ b/E-W data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mikael\Documents\Zimanyi group\ZG-FSS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72CE46EC-4A82-4229-A0E2-A313E7EE18EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5307FC15-492B-46BD-BC30-4AA3ED67553C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="2940" windowWidth="20085" windowHeight="17385" xr2:uid="{65DA8866-190D-4A07-B9F8-06CAA00B3B4B}"/>
+    <workbookView xWindow="14955" yWindow="120" windowWidth="23565" windowHeight="13605" xr2:uid="{65DA8866-190D-4A07-B9F8-06CAA00B3B4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="61">
   <si>
     <t>File</t>
   </si>
@@ -208,6 +208,15 @@
   </si>
   <si>
     <t>1.015 [.985, .044]</t>
+  </si>
+  <si>
+    <t>offdiagE5W10.txt</t>
+  </si>
+  <si>
+    <t>1.206 [.122, .259]</t>
+  </si>
+  <si>
+    <t>E5W10.png</t>
   </si>
 </sst>
 </file>
@@ -647,7 +656,7 @@
   <dimension ref="A1:R70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,6 +928,23 @@
         <v>47</v>
       </c>
     </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16">
+        <v>0.45900000000000002</v>
+      </c>
+      <c r="D16">
+        <v>3121</v>
+      </c>
+      <c r="E16" t="s">
+        <v>60</v>
+      </c>
+    </row>
     <row r="17" spans="9:18" x14ac:dyDescent="0.25">
       <c r="K17" s="8"/>
       <c r="L17" s="5"/>

</xml_diff>

<commit_message>
added E5W10improved data and updated E-W spreadsheet added WcPlot script
</commit_message>
<xml_diff>
--- a/E-W data.xlsx
+++ b/E-W data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mikael\Documents\Zimanyi group\ZG-FSS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5307FC15-492B-46BD-BC30-4AA3ED67553C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1EDD97-B95F-40AD-9B5E-4D280F1C9DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14955" yWindow="120" windowWidth="23565" windowHeight="13605" xr2:uid="{65DA8866-190D-4A07-B9F8-06CAA00B3B4B}"/>
+    <workbookView xWindow="16965" yWindow="1680" windowWidth="23565" windowHeight="13605" xr2:uid="{65DA8866-190D-4A07-B9F8-06CAA00B3B4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -210,13 +210,13 @@
     <t>1.015 [.985, .044]</t>
   </si>
   <si>
-    <t>offdiagE5W10.txt</t>
-  </si>
-  <si>
-    <t>1.206 [.122, .259]</t>
-  </si>
-  <si>
     <t>E5W10.png</t>
+  </si>
+  <si>
+    <t>offdiagE5W10improved.txt</t>
+  </si>
+  <si>
+    <t>1.209 [.165, .246]</t>
   </si>
 </sst>
 </file>
@@ -930,19 +930,19 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C16">
-        <v>0.45900000000000002</v>
+        <v>0.46</v>
       </c>
       <c r="D16">
         <v>3121</v>
       </c>
       <c r="E16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="9:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
new data and new script for simulating W/t distributions
</commit_message>
<xml_diff>
--- a/E-W data.xlsx
+++ b/E-W data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mikael\Documents\Zimanyi group\ZG-FSS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1EDD97-B95F-40AD-9B5E-4D280F1C9DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E338E0AD-572B-4EF9-BC14-186CC009032D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16965" yWindow="1680" windowWidth="23565" windowHeight="13605" xr2:uid="{65DA8866-190D-4A07-B9F8-06CAA00B3B4B}"/>
+    <workbookView xWindow="18840" yWindow="1905" windowWidth="19305" windowHeight="15315" xr2:uid="{65DA8866-190D-4A07-B9F8-06CAA00B3B4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="97">
   <si>
     <t>File</t>
   </si>
@@ -217,6 +217,114 @@
   </si>
   <si>
     <t>1.209 [.165, .246]</t>
+  </si>
+  <si>
+    <t>offdiagE0W10.txt</t>
+  </si>
+  <si>
+    <t>offdiagE0W12.txt</t>
+  </si>
+  <si>
+    <t>offdiagE0W14.txt</t>
+  </si>
+  <si>
+    <t>E0W10.png</t>
+  </si>
+  <si>
+    <t>1.27 [.225, .297]</t>
+  </si>
+  <si>
+    <t>E0W14.png</t>
+  </si>
+  <si>
+    <t>1.159 [.130, .185]</t>
+  </si>
+  <si>
+    <t>E0W12.png</t>
+  </si>
+  <si>
+    <t>offdiagE0W16.txt</t>
+  </si>
+  <si>
+    <t>1.396 [.339, .464]</t>
+  </si>
+  <si>
+    <t>E0W16.png</t>
+  </si>
+  <si>
+    <t>offdiagE0W8.txt</t>
+  </si>
+  <si>
+    <t>1.133 [.088, .172]</t>
+  </si>
+  <si>
+    <t>E0W8.png</t>
+  </si>
+  <si>
+    <t>1.142 [.121, .160]</t>
+  </si>
+  <si>
+    <t>offdiagE2W8.txt</t>
+  </si>
+  <si>
+    <t>1.129 [.106, .145]</t>
+  </si>
+  <si>
+    <t>E2W8.png</t>
+  </si>
+  <si>
+    <t>offdiagE4W8.txt</t>
+  </si>
+  <si>
+    <t>1.158 [.143, .176]</t>
+  </si>
+  <si>
+    <t>E4W8.png</t>
+  </si>
+  <si>
+    <t>offdiagE6W16take2.txt</t>
+  </si>
+  <si>
+    <t>1.892 [.769, 2.04]</t>
+  </si>
+  <si>
+    <t>E6W16take2.png</t>
+  </si>
+  <si>
+    <t>offdiagE6W14take2.txt</t>
+  </si>
+  <si>
+    <t>1.366 [.339, .402]</t>
+  </si>
+  <si>
+    <t>E6W14take2.png</t>
+  </si>
+  <si>
+    <t>offdiagE4W16take2.txt</t>
+  </si>
+  <si>
+    <t>1.408 [.346, .487]</t>
+  </si>
+  <si>
+    <t>E4W16take2.png</t>
+  </si>
+  <si>
+    <t>offdiagE4W14take2.txt</t>
+  </si>
+  <si>
+    <t>1.273 [.236, .311]</t>
+  </si>
+  <si>
+    <t>E4W14take2.png</t>
+  </si>
+  <si>
+    <t>offdiagE2W16take2.txt</t>
+  </si>
+  <si>
+    <t>1.406 [.344, .471]</t>
+  </si>
+  <si>
+    <t>E2W16take2.png</t>
   </si>
 </sst>
 </file>
@@ -655,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F0B2AE2-0F71-47D0-9A8F-E14FFEC66178}">
   <dimension ref="A1:R70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,7 +1053,22 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="9:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17">
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="D17">
+        <v>3121</v>
+      </c>
+      <c r="E17" t="s">
+        <v>64</v>
+      </c>
       <c r="K17" s="8"/>
       <c r="L17" s="5"/>
       <c r="M17" s="9"/>
@@ -953,7 +1076,56 @@
       <c r="P17" s="10"/>
       <c r="Q17" s="7"/>
     </row>
-    <row r="20" spans="9:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18">
+        <v>0.432</v>
+      </c>
+      <c r="D18">
+        <v>3121</v>
+      </c>
+      <c r="E18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D19">
+        <v>3121</v>
+      </c>
+      <c r="E19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20">
+        <v>0.76</v>
+      </c>
+      <c r="D20">
+        <v>3121</v>
+      </c>
+      <c r="E20" t="s">
+        <v>71</v>
+      </c>
       <c r="K20" s="1" t="s">
         <v>19</v>
       </c>
@@ -966,7 +1138,22 @@
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
     </row>
-    <row r="21" spans="9:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="D21">
+        <v>3121</v>
+      </c>
+      <c r="E21" t="s">
+        <v>74</v>
+      </c>
       <c r="I21" t="s">
         <v>8</v>
       </c>
@@ -990,7 +1177,22 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="9:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B22" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22">
+        <v>0.186</v>
+      </c>
+      <c r="D22">
+        <v>3121</v>
+      </c>
+      <c r="E22" t="s">
+        <v>78</v>
+      </c>
       <c r="I22" t="s">
         <v>38</v>
       </c>
@@ -1014,7 +1216,22 @@
         <v>1.18</v>
       </c>
     </row>
-    <row r="23" spans="9:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="D23">
+        <v>3121</v>
+      </c>
+      <c r="E23" t="s">
+        <v>81</v>
+      </c>
       <c r="J23" s="3"/>
       <c r="K23">
         <v>0.01</v>
@@ -1035,7 +1252,22 @@
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="24" spans="9:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="D24">
+        <v>3121</v>
+      </c>
+      <c r="E24" t="s">
+        <v>84</v>
+      </c>
       <c r="J24" s="3"/>
       <c r="K24">
         <v>0.02</v>
@@ -1056,7 +1288,22 @@
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="25" spans="9:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25">
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="D25">
+        <v>3121</v>
+      </c>
+      <c r="E25" t="s">
+        <v>87</v>
+      </c>
       <c r="J25" s="3"/>
       <c r="K25">
         <v>0.03</v>
@@ -1077,7 +1324,22 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="26" spans="9:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26">
+        <v>0.78900000000000003</v>
+      </c>
+      <c r="D26">
+        <v>3121</v>
+      </c>
+      <c r="E26" t="s">
+        <v>90</v>
+      </c>
       <c r="J26" s="3"/>
       <c r="K26">
         <v>0.04</v>
@@ -1098,7 +1360,22 @@
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="27" spans="9:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27">
+        <v>0.621</v>
+      </c>
+      <c r="D27">
+        <v>3121</v>
+      </c>
+      <c r="E27" t="s">
+        <v>93</v>
+      </c>
       <c r="J27" s="3"/>
       <c r="K27">
         <v>0.05</v>
@@ -1122,13 +1399,28 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="9:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>94</v>
+      </c>
+      <c r="B28" t="s">
+        <v>95</v>
+      </c>
+      <c r="C28">
+        <v>0.76600000000000001</v>
+      </c>
+      <c r="D28">
+        <v>3121</v>
+      </c>
+      <c r="E28" t="s">
+        <v>96</v>
+      </c>
       <c r="J28" s="3"/>
     </row>
-    <row r="29" spans="9:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J29" s="3"/>
     </row>
-    <row r="30" spans="9:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="I30" t="s">
         <v>9</v>
       </c>
@@ -1152,7 +1444,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="9:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="I31" t="s">
         <v>22</v>
       </c>
@@ -1176,7 +1468,7 @@
         <v>1.19</v>
       </c>
     </row>
-    <row r="32" spans="9:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J32" s="3"/>
       <c r="K32">
         <v>0.01</v>

</xml_diff>